<commit_message>
Added ABC to master BOM. Some stuff looked sketchy so it is being left off until later
</commit_message>
<xml_diff>
--- a/Airbrake Motor Controller/Project Outputs for Airbrake Motor Controller/Airbrake Motor Controller.xlsx
+++ b/Airbrake Motor Controller/Project Outputs for Airbrake Motor Controller/Airbrake Motor Controller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshh\Desktop\MASA-D\git\2020-2021\2020-21-PCBs\Airbrake Motor Controller\Project Outputs for Airbrake Motor Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\Airbrake Motor Controller\Project Outputs for Airbrake Motor Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA9E31E8-A34C-4F44-92B5-9C1612BDCE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{874CAE61-4718-4FFE-8EFD-A7FF6ADF8815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="804" windowWidth="6036" windowHeight="9024" xr2:uid="{A459FCAD-4F50-4580-BCA3-AB99F07C88FD}"/>
+    <workbookView xWindow="7200" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{BEBF409B-0774-48C4-895E-6E42C8F278EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Airbrake Motor Controller" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="287">
   <si>
     <t>Line #</t>
   </si>
@@ -185,10 +186,7 @@
     <t>12pF</t>
   </si>
   <si>
-    <t>Newark</t>
-  </si>
-  <si>
-    <t>03AC2652</t>
+    <t>Arrow Electronics</t>
   </si>
   <si>
     <t>C8, C25, C32</t>
@@ -203,7 +201,7 @@
     <t>CL10B105MO8NNWC</t>
   </si>
   <si>
-    <t>82AC9338</t>
+    <t>1276-6524-1-ND</t>
   </si>
   <si>
     <t>C16, C34, C35</t>
@@ -230,7 +228,7 @@
     <t>CC0603KRX7R9BB681</t>
   </si>
   <si>
-    <t>Arrow Electronics</t>
+    <t>311-1188-1-ND</t>
   </si>
   <si>
     <t>C21, C26</t>
@@ -239,399 +237,393 @@
     <t>10uF</t>
   </si>
   <si>
+    <t>C0805C106K4PACTU</t>
+  </si>
+  <si>
+    <t>399-8012-1-ND</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R7BB103</t>
+  </si>
+  <si>
+    <t>311-1042-6-ND</t>
+  </si>
+  <si>
+    <t>C29</t>
+  </si>
+  <si>
+    <t>6.8nF</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>47nF</t>
+  </si>
+  <si>
+    <t>490-3896-6-ND</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>166nF</t>
+  </si>
+  <si>
+    <t>C33</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>C0402C225K9PACTU</t>
+  </si>
+  <si>
+    <t>399-11617-1-ND</t>
+  </si>
+  <si>
+    <t>Cap2</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>PCAP_8x10-ELECT_NCA</t>
+  </si>
+  <si>
+    <t>Nichicon</t>
+  </si>
+  <si>
+    <t>UWT1H101MNL1GS</t>
+  </si>
+  <si>
+    <t>493-2226-1-ND</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>Typical RED GaAs LED</t>
+  </si>
+  <si>
+    <t>D1, D4</t>
+  </si>
+  <si>
+    <t>Diode 10TQ035</t>
+  </si>
+  <si>
+    <t>Schottky Rectifier</t>
+  </si>
+  <si>
+    <t>D2, D3</t>
+  </si>
+  <si>
+    <t>TO-220AC, CFP5_SOD128_NEX</t>
+  </si>
+  <si>
+    <t>Nexperia USA</t>
+  </si>
+  <si>
+    <t>PMEG4030EP,115</t>
+  </si>
+  <si>
+    <t>1727-5841-1-ND</t>
+  </si>
+  <si>
+    <t>Thermistor Connector</t>
+  </si>
+  <si>
+    <t>No Description Available</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN_B2B-EH-A (LF)(SN)_JST</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>B2B-EH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1611-ND</t>
+  </si>
+  <si>
+    <t>Encoder Connector</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CONN_B6B-XH-A(LF)(SN)_JST</t>
+  </si>
+  <si>
+    <t>B6BXHA(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-2271-ND</t>
+  </si>
+  <si>
+    <t>B4B-XH-A (LF)(SN)</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>CONN_B4B-XH-A (LF)(SN)_JST</t>
+  </si>
+  <si>
+    <t>B4B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-2249-ND</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>3.9nH</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>HK10053N9S-T</t>
+  </si>
+  <si>
+    <t>587-1509-6-ND</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>15nH</t>
+  </si>
+  <si>
+    <t>LQG15WZ15NJ02D</t>
+  </si>
+  <si>
+    <t>490-15252-6-ND</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>744042004</t>
+  </si>
+  <si>
+    <t>SMD Shielded Tiny Power Inductor WE-TPC, L = 4.70 µH</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>CMP-0227-00330-1</t>
+  </si>
+  <si>
+    <t>4.7uH</t>
+  </si>
+  <si>
+    <t>WE-TPC-4818-M</t>
+  </si>
+  <si>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>732-1021-1-ND</t>
+  </si>
+  <si>
+    <t>74477110</t>
+  </si>
+  <si>
+    <t>SMD-Shielded Power Inductor WE-PD, L = 10.0 µH</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>CMP-0227-00708-1</t>
+  </si>
+  <si>
+    <t>WE-PD-L</t>
+  </si>
+  <si>
+    <t>732-1208-1-ND</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-L-DV-K</t>
+  </si>
+  <si>
+    <t>Male Header, Pitch 1.27 mm, 2 x 5 Position, Height 6.25 mm</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>CMP-2000-05353-1</t>
+  </si>
+  <si>
+    <t>SMTC-FTSH-105-01-L-DV-K_V</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>SAM8799-ND</t>
+  </si>
+  <si>
+    <t>Res1</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>RC0402FR-071KL</t>
+  </si>
+  <si>
+    <t>311-1.00KLRDKR-ND</t>
+  </si>
+  <si>
+    <t>R2, R3, R6, R7</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>PNM0402E5001BST1</t>
+  </si>
+  <si>
+    <t>541-1901-6-ND</t>
+  </si>
+  <si>
+    <t>R4, R5, R8, R9, R13, R16, R20, R24, R25</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>RC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>311-0.0JRDKR-ND</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1500X</t>
+  </si>
+  <si>
+    <t>P150LDKR-ND</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>150k</t>
+  </si>
+  <si>
+    <t>ERA-3AEB154V</t>
+  </si>
+  <si>
+    <t>P150KDBCT-ND</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>16.5k</t>
+  </si>
+  <si>
+    <t>ERA-2AEB1652X</t>
+  </si>
+  <si>
+    <t>P16.5KDCDKR-ND</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>78.7K</t>
+  </si>
+  <si>
+    <t>RT0402BRD0778K7L</t>
+  </si>
+  <si>
+    <t>YAG4311DKR-ND</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>1.6k</t>
+  </si>
+  <si>
+    <t>ERA-2AEB162X</t>
+  </si>
+  <si>
+    <t>P1.6KDCCT-ND</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>1.14k</t>
+  </si>
+  <si>
     <t>6-0805_N</t>
   </si>
   <si>
-    <t>C0805C106K4PACTU</t>
-  </si>
-  <si>
-    <t>36X2702</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>CC0402KRX7R7BB103</t>
-  </si>
-  <si>
-    <t>65R7669</t>
-  </si>
-  <si>
-    <t>C29</t>
-  </si>
-  <si>
-    <t>6.8nf</t>
-  </si>
-  <si>
-    <t>C0402C682K5RACTU</t>
-  </si>
-  <si>
-    <t>33AH0961</t>
-  </si>
-  <si>
-    <t>C30</t>
-  </si>
-  <si>
-    <t>47nF</t>
-  </si>
-  <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>166nF</t>
-  </si>
-  <si>
-    <t>C33</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>C0402C225K9PACTU</t>
-  </si>
-  <si>
-    <t>96Y6898</t>
-  </si>
-  <si>
-    <t>Cap2</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>100uF</t>
-  </si>
-  <si>
-    <t>PCAP_8x10-ELECT_NCA</t>
-  </si>
-  <si>
-    <t>Nichicon</t>
-  </si>
-  <si>
-    <t>UWT1H101MNL1GS</t>
-  </si>
-  <si>
-    <t>493-2226-1-ND</t>
-  </si>
-  <si>
-    <t>LED1</t>
-  </si>
-  <si>
-    <t>Typical RED GaAs LED</t>
-  </si>
-  <si>
-    <t>D1, D4</t>
-  </si>
-  <si>
-    <t>Diode 10TQ035</t>
-  </si>
-  <si>
-    <t>Schottky Rectifier</t>
-  </si>
-  <si>
-    <t>D2, D3</t>
-  </si>
-  <si>
-    <t>TO-220AC, CFP5_SOD128_NEX</t>
-  </si>
-  <si>
-    <t>Nexperia USA</t>
-  </si>
-  <si>
-    <t>PMEG4030EP,115</t>
-  </si>
-  <si>
-    <t>Farnell</t>
-  </si>
-  <si>
-    <t>1829201</t>
-  </si>
-  <si>
-    <t>Thermistor Connector</t>
-  </si>
-  <si>
-    <t>No Description Available</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>CONN_B2B-EH-A (LF)(SN)_JST</t>
-  </si>
-  <si>
-    <t>JST</t>
-  </si>
-  <si>
-    <t>B2B-EH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>455-1611-ND</t>
-  </si>
-  <si>
-    <t>Encoder Connector</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>CONN_B6B-XH-A(LF)(SN)_JST</t>
-  </si>
-  <si>
-    <t>B6BXHA(LF)(SN)</t>
-  </si>
-  <si>
-    <t>Future Electronics</t>
-  </si>
-  <si>
-    <t>3842853</t>
-  </si>
-  <si>
-    <t>B4B-XH-A (LF)(SN)</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>CONN_B4B-XH-A (LF)(SN)_JST</t>
-  </si>
-  <si>
-    <t>B4B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>455-2249-ND</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>3.9nH</t>
-  </si>
-  <si>
-    <t>Taiyo Yuden</t>
-  </si>
-  <si>
-    <t>HK10053N9S-T</t>
-  </si>
-  <si>
-    <t>Mouser</t>
-  </si>
-  <si>
-    <t>963-HK10053N9S-T</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>15nH</t>
-  </si>
-  <si>
-    <t>LQG15WZ15NJ02D</t>
-  </si>
-  <si>
-    <t>490-15252-6-ND</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>10uH</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>MLZ1608N100LT000</t>
-  </si>
-  <si>
-    <t>445-6755-6-ND</t>
-  </si>
-  <si>
-    <t>744042004</t>
-  </si>
-  <si>
-    <t>SMD Shielded Tiny Power Inductor WE-TPC, L = 4.70 µH</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>CMP-0227-00330-1</t>
-  </si>
-  <si>
-    <t>WE-TPC-4818-M</t>
-  </si>
-  <si>
-    <t>Wurth Electronics</t>
-  </si>
-  <si>
-    <t>732-1021-1-ND</t>
-  </si>
-  <si>
-    <t>74477110</t>
-  </si>
-  <si>
-    <t>SMD-Shielded Power Inductor WE-PD, L = 10.0 µH</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>CMP-0227-00708-1</t>
-  </si>
-  <si>
-    <t>WE-PD-L</t>
-  </si>
-  <si>
-    <t>732-1208-1-ND</t>
-  </si>
-  <si>
-    <t>FTSH-105-01-L-DV-K</t>
-  </si>
-  <si>
-    <t>Male Header, Pitch 1.27 mm, 2 x 5 Position, Height 6.25 mm</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>CMP-2000-05353-1</t>
-  </si>
-  <si>
-    <t>SMTC-FTSH-105-01-L-DV-K_V</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>SAM8799-ND</t>
-  </si>
-  <si>
-    <t>Res1</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>RC0402JR-070RL</t>
-  </si>
-  <si>
-    <t>45Y6899</t>
-  </si>
-  <si>
-    <t>R2, R3, R6, R7</t>
-  </si>
-  <si>
-    <t>5k</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>PNM0402E5001BST1</t>
-  </si>
-  <si>
-    <t>541-1901-6-ND</t>
-  </si>
-  <si>
-    <t>R4, R5, R8, R9, R13, R16, R20, R24, R25</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>RC0402FR-071KL</t>
-  </si>
-  <si>
-    <t>48Y4534</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>ERJ-2RKF1500X</t>
-  </si>
-  <si>
-    <t>90W2977</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>150k</t>
-  </si>
-  <si>
-    <t>ERA-3AEB154V</t>
-  </si>
-  <si>
-    <t>08N2104</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>16.5k</t>
-  </si>
-  <si>
-    <t>ERA-2AEB1652X</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>78.7K</t>
-  </si>
-  <si>
-    <t>RT0402BRD0778K7L</t>
-  </si>
-  <si>
-    <t>YAG4311DKR-ND</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>1.6k</t>
-  </si>
-  <si>
-    <t>ERA-2AEB162X</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>1.14k</t>
-  </si>
-  <si>
     <t>ERJ-PB6B1131V</t>
   </si>
   <si>
@@ -653,7 +645,7 @@
     <t>ESR10EZPJ681</t>
   </si>
   <si>
-    <t>755-ESR10EZPJ681</t>
+    <t>RHM680KDKR-ND</t>
   </si>
   <si>
     <t>R22, R23</t>
@@ -686,6 +678,9 @@
     <t>MCS04020C1004FE000</t>
   </si>
   <si>
+    <t>MCS0402-1.00M-CFCT-ND</t>
+  </si>
+  <si>
     <t>NRF52832-QFAA-R</t>
   </si>
   <si>
@@ -782,7 +777,7 @@
     <t>Monolithic Power Systems</t>
   </si>
   <si>
-    <t>946-MP5087GG-Z</t>
+    <t>1589-1695-6-ND</t>
   </si>
   <si>
     <t>TPS55340-Q1</t>
@@ -824,18 +819,18 @@
     <t>ACS70331EESATR-005U3</t>
   </si>
   <si>
+    <t>Current Sensor 5A 1 Channel Hall Effect, Open Loop Unidirectional 12-PowerWQFN</t>
+  </si>
+  <si>
     <t>U8</t>
   </si>
   <si>
-    <t>QFN-12_ALM</t>
+    <t>ALLEGRO_ACS70331EESATR-005U3</t>
   </si>
   <si>
     <t>Allegro MicroSystems</t>
   </si>
   <si>
-    <t>620-1888-6-ND</t>
-  </si>
-  <si>
     <t>DRV8825PWP</t>
   </si>
   <si>
@@ -902,7 +897,7 @@
     <t>B2P-VH-(LF)(SN)</t>
   </si>
   <si>
-    <t>B2P-VH (LF) (SN)</t>
+    <t>455-1639-ND</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDA2CF1-6E80-46FD-A4B4-8EE2CF4B3D70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5E2273-8936-4B71-A0EE-06F1B310C72B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1292,25 +1287,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.21875" customWidth="1"/>
-    <col min="13" max="13" width="21.88671875" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1399,10 +1394,10 @@
         <v>0.51</v>
       </c>
       <c r="O2" s="4">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1444,10 +1439,10 @@
         <v>0.1</v>
       </c>
       <c r="O3" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1478,7 +1473,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1520,10 +1515,10 @@
         <v>0.1</v>
       </c>
       <c r="O5" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1562,13 +1557,13 @@
         <v>46</v>
       </c>
       <c r="N6" s="4">
-        <v>0.188</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="O6" s="4">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1604,16 +1599,16 @@
         <v>49</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N7" s="4">
-        <v>6.3E-2</v>
+        <v>8.9300000000000004E-2</v>
       </c>
       <c r="O7" s="4">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.62509999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1624,41 +1619,41 @@
         <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4">
         <v>3</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="N8" s="4">
-        <v>8.0000000000000002E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O8" s="4">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1669,41 +1664,41 @@
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4">
         <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="N9" s="4">
-        <v>8.1000000000000003E-2</v>
+        <v>0.11</v>
       </c>
       <c r="O9" s="4">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1714,14 +1709,14 @@
         <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>43</v>
@@ -1730,25 +1725,25 @@
         <v>38</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="N10" s="4">
-        <v>4.3900000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="O10" s="4">
-        <v>0.13170000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1759,41 +1754,41 @@
         <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4">
         <v>2</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N11" s="4">
-        <v>7.0999999999999994E-2</v>
+        <v>0.2</v>
       </c>
       <c r="O11" s="4">
-        <v>0.42599999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1804,14 +1799,14 @@
         <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>29</v>
@@ -1820,25 +1815,25 @@
         <v>38</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N12" s="4">
-        <v>6.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O12" s="4">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -1847,41 +1842,27 @@
         <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0.04</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1892,14 +1873,14 @@
         <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>29</v>
@@ -1914,19 +1895,19 @@
         <v>22</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="N14" s="4">
-        <v>6.3E-2</v>
+        <v>0.34</v>
       </c>
       <c r="O14" s="4">
-        <v>0.189</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1937,14 +1918,14 @@
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>29</v>
@@ -1959,19 +1940,19 @@
         <v>22</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="N15" s="4">
-        <v>6.3E-2</v>
+        <v>0.34</v>
       </c>
       <c r="O15" s="4">
-        <v>0.189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1982,14 +1963,14 @@
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4">
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>29</v>
@@ -1998,81 +1979,81 @@
         <v>30</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N16" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.2</v>
       </c>
       <c r="O16" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4">
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="K17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="N17" s="4">
         <v>0.44</v>
       </c>
       <c r="O17" s="4">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4">
@@ -2090,18 +2071,18 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4">
@@ -2109,42 +2090,42 @@
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0.43</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0.40688000000000002</v>
-      </c>
-      <c r="O19" s="4">
-        <v>2.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4">
@@ -2152,13 +2133,13 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>22</v>
@@ -2167,27 +2148,27 @@
         <v>23</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N20" s="4">
         <v>0.14000000000000001</v>
       </c>
       <c r="O20" s="4">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
@@ -2195,42 +2176,42 @@
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="N21" s="4">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="O21" s="4">
-        <v>0.54300000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4">
@@ -2238,13 +2219,13 @@
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>22</v>
@@ -2253,79 +2234,79 @@
         <v>23</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="N22" s="4">
         <v>0.21</v>
       </c>
       <c r="O22" s="4">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
         <v>2</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="N23" s="4">
-        <v>2.1999999999999999E-2</v>
+        <v>0.1</v>
       </c>
       <c r="O23" s="4">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>29</v>
@@ -2334,7 +2315,7 @@
         <v>44</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>32</v>
@@ -2343,131 +2324,137 @@
         <v>23</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N24" s="4">
         <v>0.13</v>
       </c>
       <c r="O24" s="4">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4">
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.13389999999999999</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0.13389999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="N25" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="O25" s="4">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3" t="s">
+      <c r="J26" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="N26" s="4">
         <v>1.43</v>
       </c>
       <c r="O26" s="4">
-        <v>4.29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="H27" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>22</v>
@@ -2476,79 +2463,79 @@
         <v>23</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="N27" s="4">
         <v>2.12</v>
       </c>
       <c r="O27" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="N28" s="4">
-        <v>3.13</v>
+        <v>2.87</v>
       </c>
       <c r="O28" s="4">
-        <v>9.39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4">
         <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>29</v>
@@ -2557,52 +2544,52 @@
         <v>38</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="N29" s="4">
-        <v>2E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O29" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
         <v>4</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>22</v>
@@ -2611,34 +2598,34 @@
         <v>23</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="N30" s="4">
-        <v>0.86799999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="O30" s="4">
-        <v>10.42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4">
         <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>29</v>
@@ -2647,7 +2634,7 @@
         <v>38</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>22</v>
@@ -2656,34 +2643,34 @@
         <v>23</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="N31" s="4">
         <v>1.4E-2</v>
       </c>
       <c r="O31" s="4">
-        <v>0.378</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4">
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>29</v>
@@ -2692,174 +2679,178 @@
         <v>38</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="N32" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O32" s="4">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4">
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="N33" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
       <c r="O33" s="4">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="J34" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="N34" s="4">
-        <v>3.2000000000000001E-2</v>
+        <v>0.31</v>
       </c>
       <c r="O34" s="4">
-        <v>9.6000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="N35" s="4">
-        <v>0.35849999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="O35" s="4">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B36" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>29</v>
@@ -2868,7 +2859,7 @@
         <v>38</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>22</v>
@@ -2877,311 +2868,313 @@
         <v>23</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="N36" s="4">
         <v>0.38</v>
       </c>
       <c r="O36" s="4">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="N37" s="4">
-        <v>6.88E-2</v>
+        <v>0.39</v>
       </c>
       <c r="O37" s="4">
-        <v>0.2064</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="N38" s="4">
         <v>0.33</v>
       </c>
       <c r="O38" s="4">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B39" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="N39" s="4">
         <v>0.1</v>
       </c>
       <c r="O39" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
         <v>2</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="K40" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="L40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="N40" s="4">
         <v>0.63</v>
       </c>
       <c r="O40" s="4">
-        <v>3.78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>29</v>
       </c>
       <c r="I41" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="N41" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="O41" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="N41" s="4">
-        <v>0.18110000000000001</v>
-      </c>
-      <c r="O41" s="4">
-        <v>0.54330000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="F42" s="4">
         <v>1</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="N42" s="4">
         <v>5.46</v>
       </c>
       <c r="O42" s="4">
-        <v>16.38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="F43" s="4">
         <v>1</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>32</v>
@@ -3190,117 +3183,117 @@
         <v>23</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N43" s="4">
         <v>0.9</v>
       </c>
       <c r="O43" s="4">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M44" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="N44" s="4">
         <v>2.92</v>
       </c>
       <c r="O44" s="4">
-        <v>8.76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M45" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="N45" s="4">
         <v>1.69</v>
       </c>
       <c r="O45" s="4">
-        <v>5.07</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4">
@@ -3308,42 +3301,42 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M46" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="N46" s="4">
+        <v>1.29</v>
+      </c>
+      <c r="O46" s="4">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="J46" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="M46" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="N46" s="4">
-        <v>1.28</v>
-      </c>
-      <c r="O46" s="4">
-        <v>3.84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4">
@@ -3351,87 +3344,87 @@
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="N47" s="4">
         <v>4.5999999999999996</v>
       </c>
       <c r="O47" s="4">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="F48" s="4">
         <v>1</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M48" s="3" t="s">
-        <v>260</v>
       </c>
       <c r="N48" s="4">
         <v>0.44</v>
       </c>
       <c r="O48" s="4">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4">
@@ -3439,58 +3432,50 @@
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="I49" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="J49" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L49" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M49" s="3" t="s">
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="N49" s="4">
-        <v>1.87</v>
-      </c>
-      <c r="O49" s="4">
-        <v>5.61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="144" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
       </c>
       <c r="G50" s="4"/>
       <c r="H50" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K50" s="3" t="s">
         <v>22</v>
@@ -3499,27 +3484,27 @@
         <v>23</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N50" s="4">
         <v>5.09</v>
       </c>
       <c r="O50" s="4">
-        <v>15.27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4">
@@ -3527,38 +3512,38 @@
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="J51" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="I51" s="3" t="s">
+      <c r="K51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M51" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
     </row>
-    <row r="52" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4">
@@ -3566,13 +3551,13 @@
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K52" s="3" t="s">
         <v>32</v>
@@ -3581,27 +3566,27 @@
         <v>23</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N52" s="4">
         <v>0.44</v>
       </c>
       <c r="O52" s="4">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4">
@@ -3609,33 +3594,33 @@
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M53" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="I53" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="N53" s="4">
-        <v>0.17030000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="O53" s="4">
-        <v>0.51090000000000002</v>
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="25" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="24" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed minor BOM errors
</commit_message>
<xml_diff>
--- a/Airbrake Motor Controller/Project Outputs for Airbrake Motor Controller/Airbrake Motor Controller.xlsx
+++ b/Airbrake Motor Controller/Project Outputs for Airbrake Motor Controller/Airbrake Motor Controller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\Airbrake Motor Controller\Project Outputs for Airbrake Motor Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9F9F7A-CE50-4620-8B22-134BCD851DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C7F77FA-E3E9-4B89-ADEE-ED650A373E8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Diode 10TQ035</t>
   </si>
   <si>
-    <t>Thermistor Connector</t>
+    <t>B2B-EH-A (LF)(SN)</t>
   </si>
   <si>
     <t>Encoder Connector</t>
@@ -87,7 +87,7 @@
     <t>MP5087GG</t>
   </si>
   <si>
-    <t>TPS55340-Q1</t>
+    <t>TPS55340QRTERQ1</t>
   </si>
   <si>
     <t>AP2204K-5.0TRG1</t>
@@ -282,9 +282,6 @@
     <t>MP5087GG-Z</t>
   </si>
   <si>
-    <t>TPS55340QRTETQ1</t>
-  </si>
-  <si>
     <t>FC-13532.7680KA-AC</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
   </si>
   <si>
     <t>DDC0006A_L</t>
-  </si>
-  <si>
-    <t>TPS55340QRTERQ1</t>
   </si>
   <si>
     <t>FP-SOT25-IPC_B</t>
@@ -857,19 +851,19 @@
         <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -886,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2">
         <v>0.51</v>
@@ -909,10 +903,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G3">
         <v>0.1</v>
@@ -932,10 +926,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,10 +946,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5">
         <v>0.1</v>
@@ -978,10 +972,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6">
         <v>2.7E-2</v>
@@ -1004,10 +998,10 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G7">
         <v>1.35E-2</v>
@@ -1030,10 +1024,10 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8">
         <v>0.1</v>
@@ -1053,19 +1047,19 @@
         <v>49</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H9">
-        <v>0.28799999999999998</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,10 +1076,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G10">
         <v>0.1</v>
@@ -1105,19 +1099,19 @@
         <v>51</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G11">
         <v>0.16350000000000001</v>
       </c>
       <c r="H11">
-        <v>0.32700000000000001</v>
+        <v>0.8175</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1134,10 +1128,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G12">
         <v>0.1</v>
@@ -1160,16 +1154,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
       </c>
       <c r="H13">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1186,10 +1180,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G14">
         <v>3.5999999999999997E-2</v>
@@ -1212,10 +1206,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G15">
         <v>6.25E-2</v>
@@ -1238,10 +1232,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G16">
         <v>0.35</v>
@@ -1264,10 +1258,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G17">
         <v>0.44</v>
@@ -1290,10 +1284,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G18">
         <v>1.35E-2</v>
@@ -1313,7 +1307,7 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19">
         <v>0.14000000000000001</v>
@@ -1336,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20">
         <v>0.42409999999999998</v>
@@ -1359,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21">
         <v>0.14000000000000001</v>
@@ -1382,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G22">
         <v>0.27</v>
@@ -1405,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23">
         <v>0.21</v>
@@ -1428,10 +1422,10 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G24">
         <v>0.1</v>
@@ -1454,10 +1448,10 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G25">
         <v>5.5899999999999998E-2</v>
@@ -1480,10 +1474,10 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G26">
         <v>0.1341</v>
@@ -1506,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G27">
         <v>1.43</v>
@@ -1532,10 +1526,10 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G28">
         <v>2.12</v>
@@ -1558,13 +1552,13 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G29">
-        <v>2.87</v>
+        <v>2.85</v>
       </c>
       <c r="H29">
-        <v>2.87</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,10 +1575,10 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G30">
         <v>0.1</v>
@@ -1607,10 +1601,10 @@
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G31">
         <v>0.97660000000000002</v>
@@ -1633,10 +1627,10 @@
         <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G32">
         <v>1.4E-2</v>
@@ -1659,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1685,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34">
         <v>330</v>
@@ -1711,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F35">
         <v>150</v>
@@ -1737,10 +1731,10 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G36">
         <v>0.1</v>
@@ -1763,10 +1757,10 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G37">
         <v>0.39</v>
@@ -1789,10 +1783,10 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G38">
         <v>9.5899999999999999E-2</v>
@@ -1815,10 +1809,10 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G39">
         <v>0.39</v>
@@ -1841,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G40">
         <v>0.33</v>
@@ -1867,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F41">
         <v>680</v>
@@ -1893,10 +1887,10 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G42">
         <v>0.63</v>
@@ -1919,10 +1913,10 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G43">
         <v>0.26</v>
@@ -1945,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G44">
         <v>5.46</v>
@@ -1968,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45">
         <v>0.9</v>
@@ -1991,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G46">
         <v>2.92</v>
@@ -2014,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G47">
         <v>1.69</v>
@@ -2048,19 +2042,19 @@
         <v>17</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="G49">
-        <v>4.5999999999999996</v>
+        <v>3.96</v>
       </c>
       <c r="H49">
-        <v>4.5999999999999996</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2077,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G50">
         <v>0.44</v>
@@ -2100,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2117,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G52">
         <v>5.09</v>
@@ -2134,13 +2128,13 @@
         <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2174,13 +2168,13 @@
         <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G55">
         <v>0.19</v>

</xml_diff>